<commit_message>
Add one point for interactivity
Grading got changed
</commit_message>
<xml_diff>
--- a/GradedExercise.xlsx
+++ b/GradedExercise.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianr/Temp/FS19 Christian Ribeaud Graded Exercise-05-23-2019-11-26-22/NatSennrich/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianr/Temp/fs19-de-cr-graded-exercise-NatSennrich/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01A0E44-D989-3D44-8A6B-41E0C239CFA4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6375F150-5892-8544-9FD4-228B27D7BE77}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3160" yWindow="460" windowWidth="30440" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -810,7 +810,7 @@
         <v>7</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
@@ -836,11 +836,11 @@
       </c>
       <c r="G14" s="3">
         <f>SUM(G8:G13)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H14" s="3">
         <f>MIN(C14,G14)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
@@ -1036,7 +1036,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="10">
         <f>SUM(H4:H30)</f>
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
@@ -1098,7 +1098,7 @@
       <c r="H40" s="9"/>
       <c r="I40" s="9">
         <f>Bonus-Malus</f>
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
@@ -1113,7 +1113,7 @@
       <c r="H42" s="4"/>
       <c r="I42" s="5">
         <f>1 + TOTAL/10</f>
-        <v>5.9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>